<commit_message>
Add CSV vs Excel mismatch detection script and update tasks
</commit_message>
<xml_diff>
--- a/validation_reports/Snowflake_SQL_Results_20251103_202802.xlsx
+++ b/validation_reports/Snowflake_SQL_Results_20251103_202802.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvarshney\PowerBI_Automation_POM\validation_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E0CD23-AF99-4FE9-95D6-F96A4D7BFC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10844D5-7241-4885-808E-A414D39E87FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="22" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2042,6 +2042,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -5958,6 +5961,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="4" max="4" width="26.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -6537,6 +6545,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -6591,8 +6604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8833,6 +8846,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>